<commit_message>
Fix typo, add category priority colorization
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/TradeStudies/Hardware.xlsx
+++ b/TradeStudies/Hardware.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\TradeStudies\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACFF166-B0A3-4552-8656-FCC75242BE21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85D3A7-2507-43CA-AE3C-90DF676867D0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="3870" xr2:uid="{D6D99C19-C2DC-4E63-B6E2-7E3BE1AE1F62}"/>
   </bookViews>
@@ -68,9 +63,6 @@
     <t>BeagleBone Black</t>
   </si>
   <si>
-    <t>BeagleBone Enahnced</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -78,6 +70,9 @@
   </si>
   <si>
     <t>Scaling Multiplier</t>
+  </si>
+  <si>
+    <t>BeagleBone Enhanced</t>
   </si>
 </sst>
 </file>
@@ -161,7 +156,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -179,9 +174,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -191,7 +183,7 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -199,73 +191,6 @@
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -292,14 +217,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F43DDE1-5E26-457E-BBD3-9B8E2CEE3F7B}" name="Table1" displayName="Table1" ref="C13:J20" totalsRowShown="0">
   <autoFilter ref="C13:J20" xr:uid="{1157F62B-3D78-4501-9545-7EF3EF0D3503}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{27820288-3BD1-40DB-AA0B-94B2A665FF7F}" name="Hardware" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DDB0BFE1-5B47-4AAC-8CB5-6483A0A83CE2}" name="Simplicity" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2DB95F8A-AED2-4EBC-9378-D2A3A7C91ECF}" name="Deterministic" dataDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{C8309E6F-8784-4993-8C8F-6774DFA30AE5}" name="Logic reliability" dataDxfId="3" dataCellStyle="Input"/>
-    <tableColumn id="5" xr3:uid="{615BB428-D329-49A3-B9B1-2C3B784963D0}" name="Familiarity" dataDxfId="2" dataCellStyle="Input"/>
-    <tableColumn id="6" xr3:uid="{68AC69E3-46EA-443E-9AE8-D954C52A0469}" name="Physical reliability" dataDxfId="1" dataCellStyle="Input"/>
-    <tableColumn id="7" xr3:uid="{DFF03A48-8540-4F0A-9680-D19C09E4668F}" name="Language options" dataDxfId="0" dataCellStyle="Input"/>
-    <tableColumn id="8" xr3:uid="{520D4C0F-328B-4103-BFED-EEF41BC0947A}" name="Total" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{27820288-3BD1-40DB-AA0B-94B2A665FF7F}" name="Hardware" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{DDB0BFE1-5B47-4AAC-8CB5-6483A0A83CE2}" name="Simplicity" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{2DB95F8A-AED2-4EBC-9378-D2A3A7C91ECF}" name="Deterministic" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{C8309E6F-8784-4993-8C8F-6774DFA30AE5}" name="Logic reliability" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{615BB428-D329-49A3-B9B1-2C3B784963D0}" name="Familiarity" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{68AC69E3-46EA-443E-9AE8-D954C52A0469}" name="Physical reliability" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{DFF03A48-8540-4F0A-9680-D19C09E4668F}" name="Language options" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{520D4C0F-328B-4103-BFED-EEF41BC0947A}" name="Total" dataDxfId="0">
       <calculatedColumnFormula>SUMPRODUCT(D14:I14,D$11:I$11)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -607,7 +532,7 @@
   <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -786,10 +711,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="8"/>
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="6">
         <v>2</v>
       </c>
@@ -820,7 +745,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -841,29 +766,29 @@
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" s="2">
@@ -875,22 +800,22 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" s="2">
@@ -902,22 +827,22 @@
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" s="2">
@@ -929,22 +854,22 @@
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>0</v>
       </c>
       <c r="J17" s="2">
@@ -956,22 +881,22 @@
       <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0</v>
-      </c>
-      <c r="I18" s="7">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>0</v>
       </c>
       <c r="J18" s="2">
@@ -983,22 +908,22 @@
       <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" s="2">
@@ -1008,24 +933,24 @@
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" s="2">
@@ -1038,6 +963,18 @@
     <mergeCell ref="A11:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:J20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:I10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1050,8 +987,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>